<commit_message>
end of night. trying to get tests to work
</commit_message>
<xml_diff>
--- a/ExcelFileFolder/VanguardDB.xlsx
+++ b/ExcelFileFolder/VanguardDB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Calculator (Beta)" sheetId="1" r:id="rId1"/>
@@ -13350,7 +13350,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
struggling against infinite looping problem
</commit_message>
<xml_diff>
--- a/ExcelFileFolder/VanguardDB.xlsx
+++ b/ExcelFileFolder/VanguardDB.xlsx
@@ -1075,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1289,7 +1289,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1305,7 +1304,9 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5672,13 +5673,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
       <c r="F1" s="2"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -5703,12 +5704,12 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="6"/>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
       <c r="F2" s="6"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -6050,13 +6051,13 @@
       <c r="Z10" s="16"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="97"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="97"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
       <c r="F11" s="31"/>
       <c r="G11" s="32"/>
       <c r="H11" s="32"/>
@@ -6081,12 +6082,12 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="31"/>
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
       <c r="F12" s="31"/>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
@@ -13178,7 +13179,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -13189,156 +13190,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="102" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="100" t="s">
         <v>245</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="100" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="100" t="s">
         <v>247</v>
       </c>
       <c r="B2" s="101">
         <v>0</v>
       </c>
-      <c r="C2" s="78">
+      <c r="C2" s="101">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="100" t="s">
         <v>247</v>
       </c>
-      <c r="B3" s="78">
+      <c r="B3" s="100">
         <v>1</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="100">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="100" t="s">
         <v>247</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="100">
         <v>2</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="100">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="100" t="s">
         <v>247</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="100">
         <v>3</v>
       </c>
-      <c r="C5" s="78">
+      <c r="C5" s="100">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="100" t="s">
         <v>247</v>
       </c>
-      <c r="B6" s="78">
+      <c r="B6" s="100">
         <v>4</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="100">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="100" t="s">
         <v>248</v>
       </c>
-      <c r="B7" s="78">
+      <c r="B7" s="100">
         <v>0</v>
       </c>
-      <c r="C7" s="78">
+      <c r="C7" s="100">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="100" t="s">
         <v>248</v>
       </c>
-      <c r="B8" s="78">
+      <c r="B8" s="100">
         <v>1</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="100">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="100" t="s">
         <v>248</v>
       </c>
-      <c r="B9" s="78">
+      <c r="B9" s="100">
         <v>2</v>
       </c>
-      <c r="C9" s="78">
+      <c r="C9" s="100">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="100" t="s">
         <v>248</v>
       </c>
-      <c r="B10" s="78">
+      <c r="B10" s="100">
         <v>3</v>
       </c>
-      <c r="C10" s="78">
+      <c r="C10" s="100">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="100" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="78">
+      <c r="B11" s="100">
         <v>0</v>
       </c>
-      <c r="C11" s="78">
+      <c r="C11" s="100">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="100" t="s">
         <v>249</v>
       </c>
-      <c r="B12" s="78">
+      <c r="B12" s="100">
         <v>1</v>
       </c>
-      <c r="C12" s="78">
+      <c r="C12" s="100">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="100" t="s">
         <v>249</v>
       </c>
-      <c r="B13" s="78">
+      <c r="B13" s="100">
         <v>2</v>
       </c>
-      <c r="C13" s="78">
+      <c r="C13" s="100">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="12.75">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="100" t="s">
         <v>249</v>
       </c>
-      <c r="B14" s="78">
+      <c r="B14" s="100">
         <v>3</v>
       </c>
-      <c r="C14" s="78">
+      <c r="C14" s="100">
         <v>6</v>
       </c>
     </row>
@@ -13358,22 +13359,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:4" s="95" customFormat="1">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:4" s="94" customFormat="1">
+      <c r="A1" s="94" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="94" t="s">
         <v>252</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="94" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="94" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>256</v>
       </c>
       <c r="B2">
@@ -13384,13 +13385,13 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="93" t="s">
         <v>255</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="95">
+      <c r="C3" s="94">
         <v>8.9</v>
       </c>
     </row>

</xml_diff>